<commit_message>
updated/corrected pattern assignments to be matching with other iterations
</commit_message>
<xml_diff>
--- a/Iter2-analysisPairs.xlsx
+++ b/Iter2-analysisPairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\Organizer\School\BachelorProject\GroundedTheoryDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A7D3DD-6844-4F53-BB10-6A9D5F868969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC59A701-250F-4F8F-8507-D0C4026FC8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArchIssuesAllEmails" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3265" uniqueCount="1693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3263" uniqueCount="1692">
   <si>
     <t>UID</t>
   </si>
@@ -4952,9 +4952,6 @@
   </si>
   <si>
     <t>CEP</t>
-  </si>
-  <si>
-    <t>Weird one. Issue doesn't seem very related to email but the patch does seem related</t>
   </si>
   <si>
     <t>Could be related, but probably is another ADD that is related to issue ADD</t>
@@ -5502,8 +5499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF74" sqref="AF74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5537,16 +5534,16 @@
         <v>8</v>
       </c>
       <c r="V1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="W1" t="s">
         <v>1688</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>1689</v>
       </c>
-      <c r="X1" t="s">
-        <v>1690</v>
-      </c>
       <c r="Y1" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -5639,7 +5636,7 @@
       </c>
       <c r="Z3">
         <f>COUNTIF(O2:O101,Y3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -5686,7 +5683,7 @@
       </c>
       <c r="Z4">
         <f>COUNTIF(O2:O101,Y4)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -5780,7 +5777,7 @@
       </c>
       <c r="Z6">
         <f>COUNTIF(O2:O101,Y6)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
@@ -5827,7 +5824,7 @@
       </c>
       <c r="Z7">
         <f>COUNTIF(O2:O101,Y7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -5953,7 +5950,7 @@
         <v>1632</v>
       </c>
       <c r="Q10" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="V10">
         <v>9</v>
@@ -5971,7 +5968,7 @@
       </c>
       <c r="Z10">
         <f>COUNTIF(O2:O101,Y10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
@@ -6050,7 +6047,7 @@
         <v>1632</v>
       </c>
       <c r="Q12" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="V12">
         <v>11</v>
@@ -6100,7 +6097,7 @@
         <v>3</v>
       </c>
       <c r="Q13" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="V13">
         <v>12</v>
@@ -6197,7 +6194,7 @@
         <v>3</v>
       </c>
       <c r="Q15" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="V15">
         <v>14</v>
@@ -6324,7 +6321,7 @@
         <v>52</v>
       </c>
       <c r="O18" s="3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="V18">
         <v>17</v>
@@ -6447,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="Q21" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="V21">
         <v>20</v>
@@ -6491,7 +6488,7 @@
       </c>
       <c r="P22" s="4"/>
       <c r="Q22" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="V22">
         <v>21</v>
@@ -6580,7 +6577,7 @@
         <v>1632</v>
       </c>
       <c r="Q24" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="V24">
         <v>23</v>
@@ -6743,7 +6740,7 @@
         <v>1632</v>
       </c>
       <c r="Q28" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="V28">
         <v>27</v>
@@ -6907,7 +6904,7 @@
       </c>
       <c r="P32" s="7"/>
       <c r="Q32" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V32">
         <v>31</v>
@@ -6951,7 +6948,7 @@
       </c>
       <c r="P33" s="7"/>
       <c r="Q33" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V33">
         <v>32</v>
@@ -6994,7 +6991,7 @@
         <v>1634</v>
       </c>
       <c r="Q34" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="V34">
         <v>33</v>
@@ -7038,7 +7035,7 @@
       </c>
       <c r="P35" s="4"/>
       <c r="Q35" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="V35">
         <v>34</v>
@@ -7122,7 +7119,7 @@
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="V37">
         <v>36</v>
@@ -7206,7 +7203,7 @@
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V39">
         <v>38</v>
@@ -7249,7 +7246,7 @@
         <v>1632</v>
       </c>
       <c r="Q40" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="V40">
         <v>39</v>
@@ -7369,10 +7366,10 @@
         <v>45</v>
       </c>
       <c r="O43" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Q43" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="V43">
         <v>42</v>
@@ -7415,7 +7412,7 @@
         <v>1634</v>
       </c>
       <c r="Q44" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="V44">
         <v>43</v>
@@ -7621,7 +7618,7 @@
         <v>1632</v>
       </c>
       <c r="Q49" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="V49">
         <v>48</v>
@@ -7704,7 +7701,7 @@
         <v>1634</v>
       </c>
       <c r="Q51" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="V51">
         <v>50</v>
@@ -7828,7 +7825,7 @@
       </c>
       <c r="P54" s="7"/>
       <c r="Q54" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V54">
         <v>53</v>
@@ -7954,7 +7951,7 @@
         <v>7</v>
       </c>
       <c r="Q57" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="V57">
         <v>56</v>
@@ -7997,7 +7994,7 @@
         <v>7</v>
       </c>
       <c r="Q58" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="V58">
         <v>57</v>
@@ -8080,7 +8077,7 @@
         <v>1634</v>
       </c>
       <c r="Q60" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="V60">
         <v>59</v>
@@ -8126,7 +8123,7 @@
         <v>1632</v>
       </c>
       <c r="Q61" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="V61">
         <v>60</v>
@@ -8170,7 +8167,7 @@
       </c>
       <c r="P62" s="7"/>
       <c r="Q62" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="V62">
         <v>61</v>
@@ -8334,7 +8331,7 @@
       </c>
       <c r="P66" s="8"/>
       <c r="Q66" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="V66">
         <v>65</v>
@@ -8418,7 +8415,7 @@
       </c>
       <c r="P68" s="8"/>
       <c r="Q68" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="V68">
         <v>67</v>
@@ -8461,7 +8458,7 @@
         <v>1634</v>
       </c>
       <c r="Q69" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="V69">
         <v>68</v>
@@ -8584,7 +8581,7 @@
         <v>1634</v>
       </c>
       <c r="Q72" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="V72">
         <v>71</v>
@@ -8623,20 +8620,19 @@
       <c r="M73" t="s">
         <v>144</v>
       </c>
-      <c r="O73" s="6" t="s">
-        <v>1634</v>
-      </c>
-      <c r="P73" s="7"/>
+      <c r="O73" s="3">
+        <v>6</v>
+      </c>
       <c r="V73">
         <v>72</v>
       </c>
       <c r="W73">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X73">
         <f t="shared" si="4"/>
-        <v>0.54166666666666663</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.3">
@@ -8672,11 +8668,11 @@
       </c>
       <c r="W74">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X74">
         <f t="shared" si="4"/>
-        <v>0.53424657534246578</v>
+        <v>0.54794520547945202</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
@@ -8713,11 +8709,11 @@
       </c>
       <c r="W75">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X75">
         <f t="shared" si="4"/>
-        <v>0.54054054054054057</v>
+        <v>0.55405405405405406</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.3">
@@ -8749,18 +8745,18 @@
         <v>1632</v>
       </c>
       <c r="Q76" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="V76">
         <v>75</v>
       </c>
       <c r="W76">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X76">
         <f t="shared" si="4"/>
-        <v>0.53333333333333333</v>
+        <v>0.54666666666666663</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.3">
@@ -8796,11 +8792,11 @@
       </c>
       <c r="W77">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X77">
         <f t="shared" si="4"/>
-        <v>0.52631578947368418</v>
+        <v>0.53947368421052633</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.3">
@@ -8836,11 +8832,11 @@
       </c>
       <c r="W78">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X78">
         <f t="shared" si="4"/>
-        <v>0.53246753246753242</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.3">
@@ -8876,11 +8872,11 @@
       </c>
       <c r="W79">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X79">
         <f t="shared" si="4"/>
-        <v>0.52564102564102566</v>
+        <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.3">
@@ -8916,11 +8912,11 @@
       </c>
       <c r="W80">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X80">
         <f t="shared" si="4"/>
-        <v>0.53164556962025311</v>
+        <v>0.54430379746835444</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.3">
@@ -8956,11 +8952,11 @@
       </c>
       <c r="W81">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X81">
         <f t="shared" si="4"/>
-        <v>0.52500000000000002</v>
+        <v>0.53749999999999998</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.3">
@@ -8996,11 +8992,11 @@
       </c>
       <c r="W82">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X82">
         <f t="shared" si="4"/>
-        <v>0.51851851851851849</v>
+        <v>0.53086419753086422</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.3">
@@ -9036,11 +9032,11 @@
       </c>
       <c r="W83">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X83">
         <f t="shared" si="4"/>
-        <v>0.51219512195121952</v>
+        <v>0.52439024390243905</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.3">
@@ -9073,18 +9069,18 @@
       </c>
       <c r="P84" s="7"/>
       <c r="Q84" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="V84">
         <v>83</v>
       </c>
       <c r="W84">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X84">
         <f t="shared" si="4"/>
-        <v>0.50602409638554213</v>
+        <v>0.51807228915662651</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.3">
@@ -9116,18 +9112,18 @@
         <v>1634</v>
       </c>
       <c r="Q85" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="V85">
         <v>84</v>
       </c>
       <c r="W85">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X85">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.51190476190476186</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.3">
@@ -9163,11 +9159,11 @@
       </c>
       <c r="W86">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X86">
         <f t="shared" si="4"/>
-        <v>0.49411764705882355</v>
+        <v>0.50588235294117645</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.3">
@@ -9203,11 +9199,11 @@
       </c>
       <c r="W87">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X87">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.51162790697674421</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.3">
@@ -9243,11 +9239,11 @@
       </c>
       <c r="W88">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X88">
         <f t="shared" si="4"/>
-        <v>0.4942528735632184</v>
+        <v>0.50574712643678166</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.3">
@@ -9284,11 +9280,11 @@
       </c>
       <c r="W89">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X89">
         <f t="shared" si="4"/>
-        <v>0.48863636363636365</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.3">
@@ -9324,11 +9320,11 @@
       </c>
       <c r="W90">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X90">
         <f t="shared" si="4"/>
-        <v>0.48314606741573035</v>
+        <v>0.4943820224719101</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.3">
@@ -9361,18 +9357,18 @@
       </c>
       <c r="P91" s="7"/>
       <c r="Q91" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="V91">
         <v>90</v>
       </c>
       <c r="W91">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X91">
         <f t="shared" si="4"/>
-        <v>0.4777777777777778</v>
+        <v>0.48888888888888887</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.3">
@@ -9408,11 +9404,11 @@
       </c>
       <c r="W92">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X92">
         <f t="shared" si="4"/>
-        <v>0.47252747252747251</v>
+        <v>0.48351648351648352</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.3">
@@ -9448,11 +9444,11 @@
       </c>
       <c r="W93">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X93">
         <f t="shared" si="4"/>
-        <v>0.46739130434782611</v>
+        <v>0.47826086956521741</v>
       </c>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.3">
@@ -9488,11 +9484,11 @@
       </c>
       <c r="W94">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X94">
         <f t="shared" si="4"/>
-        <v>0.46236559139784944</v>
+        <v>0.4731182795698925</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.3">
@@ -9528,11 +9524,11 @@
       </c>
       <c r="W95">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X95">
         <f t="shared" si="4"/>
-        <v>0.45744680851063829</v>
+        <v>0.46808510638297873</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.3">
@@ -9569,11 +9565,11 @@
       </c>
       <c r="W96">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X96">
         <f t="shared" si="4"/>
-        <v>0.45263157894736844</v>
+        <v>0.4631578947368421</v>
       </c>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.3">
@@ -9609,11 +9605,11 @@
       </c>
       <c r="W97">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X97">
         <f t="shared" si="4"/>
-        <v>0.44791666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.3">
@@ -9649,11 +9645,11 @@
       </c>
       <c r="W98">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X98">
         <f t="shared" si="4"/>
-        <v>0.44329896907216493</v>
+        <v>0.45360824742268041</v>
       </c>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.3">
@@ -9689,11 +9685,11 @@
       </c>
       <c r="W99">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X99">
         <f t="shared" si="4"/>
-        <v>0.43877551020408162</v>
+        <v>0.44897959183673469</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.3">
@@ -9729,11 +9725,11 @@
       </c>
       <c r="W100">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X100">
         <f t="shared" si="4"/>
-        <v>0.43434343434343436</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.3">
@@ -9769,11 +9765,11 @@
       </c>
       <c r="W101">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X101">
         <f t="shared" si="4"/>
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.3">
@@ -9965,7 +9961,7 @@
       </c>
       <c r="P108" s="7"/>
       <c r="Q108" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.3">
@@ -10413,7 +10409,7 @@
         <v>1632</v>
       </c>
       <c r="Q125" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.3">
@@ -10445,7 +10441,7 @@
         <v>1632</v>
       </c>
       <c r="Q126" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.3">
@@ -10768,7 +10764,7 @@
       </c>
       <c r="P138" s="7"/>
       <c r="Q138" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.3">
@@ -12344,7 +12340,7 @@
       </c>
       <c r="P198" s="7"/>
       <c r="Q198" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.3">
@@ -14917,7 +14913,7 @@
       </c>
       <c r="P296" s="7"/>
       <c r="Q296" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="297" spans="1:17" x14ac:dyDescent="0.3">
@@ -15106,7 +15102,7 @@
       </c>
       <c r="P303" s="7"/>
       <c r="Q303" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="304" spans="1:17" x14ac:dyDescent="0.3">
@@ -15271,7 +15267,7 @@
         <v>1632</v>
       </c>
       <c r="Q309" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="310" spans="1:17" x14ac:dyDescent="0.3">
@@ -17213,7 +17209,7 @@
         <v>7</v>
       </c>
       <c r="Q383" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="384" spans="1:17" x14ac:dyDescent="0.3">
@@ -17297,7 +17293,7 @@
         <v>1634</v>
       </c>
       <c r="Q386" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="387" spans="1:17" x14ac:dyDescent="0.3">
@@ -18583,7 +18579,7 @@
         <v>1634</v>
       </c>
       <c r="Q435" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="436" spans="1:17" x14ac:dyDescent="0.3">
@@ -20312,8 +20308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CCD5B3-028A-4A0C-BDA3-C24CA609BB7B}">
   <dimension ref="A1:Z501"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20347,16 +20343,16 @@
         <v>8</v>
       </c>
       <c r="V1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="W1" t="s">
         <v>1688</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>1689</v>
       </c>
-      <c r="X1" t="s">
-        <v>1690</v>
-      </c>
       <c r="Y1" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -20496,7 +20492,7 @@
       </c>
       <c r="Z4">
         <f>COUNTIF(O2:O101,Y4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -20546,7 +20542,7 @@
       </c>
       <c r="Z5">
         <f>COUNTIF(O2:O101,Y5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -20643,7 +20639,7 @@
       </c>
       <c r="Z7">
         <f>COUNTIF(O2:O101,Y7)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -20887,7 +20883,7 @@
       </c>
       <c r="Z12">
         <f>COUNTIF(O2:O101,Y12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
@@ -20937,7 +20933,7 @@
       </c>
       <c r="Z13">
         <f>COUNTIF(O2:O101,Y13)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -21015,22 +21011,19 @@
       <c r="M15" t="s">
         <v>89</v>
       </c>
-      <c r="O15" s="4">
-        <v>3</v>
-      </c>
-      <c r="P15" t="s">
-        <v>1637</v>
+      <c r="O15" s="6" t="s">
+        <v>1634</v>
       </c>
       <c r="V15">
         <v>14</v>
       </c>
       <c r="W15">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X15">
         <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="Y15">
         <v>16</v>
@@ -21073,11 +21066,11 @@
       </c>
       <c r="W16">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X16">
         <f t="shared" si="1"/>
-        <v>0.8666666666666667</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
@@ -21113,11 +21106,11 @@
       </c>
       <c r="W17">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X17">
         <f t="shared" si="1"/>
-        <v>0.875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
@@ -21153,11 +21146,11 @@
       </c>
       <c r="W18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X18">
         <f t="shared" si="1"/>
-        <v>0.88235294117647056</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
@@ -21196,11 +21189,11 @@
       </c>
       <c r="W19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X19">
         <f t="shared" si="1"/>
-        <v>0.88888888888888884</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
@@ -21228,22 +21221,19 @@
       <c r="M20" t="s">
         <v>213</v>
       </c>
-      <c r="O20" s="4">
-        <v>14</v>
-      </c>
-      <c r="P20" s="6" t="s">
+      <c r="O20" s="6" t="s">
         <v>1634</v>
       </c>
       <c r="V20">
         <v>19</v>
       </c>
       <c r="W20">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>W19+(IF(ISNUMBER(#REF!),1,0))</f>
+        <v>15</v>
       </c>
       <c r="X20">
         <f t="shared" si="1"/>
-        <v>0.89473684210526316</v>
+        <v>0.78947368421052633</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
@@ -21279,11 +21269,11 @@
       </c>
       <c r="W21">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="X21">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -21322,11 +21312,11 @@
       </c>
       <c r="W22">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X22">
         <f t="shared" si="1"/>
-        <v>0.90476190476190477</v>
+        <v>0.80952380952380953</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
@@ -21359,18 +21349,18 @@
       </c>
       <c r="P23" s="7"/>
       <c r="Q23" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V23">
         <v>22</v>
       </c>
       <c r="W23">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X23">
         <f t="shared" si="1"/>
-        <v>0.86363636363636365</v>
+        <v>0.77272727272727271</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
@@ -21406,11 +21396,11 @@
       </c>
       <c r="W24">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X24">
         <f t="shared" si="1"/>
-        <v>0.82608695652173914</v>
+        <v>0.73913043478260865</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
@@ -21446,11 +21436,11 @@
       </c>
       <c r="W25">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="X25">
         <f t="shared" si="1"/>
-        <v>0.79166666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -21486,11 +21476,11 @@
       </c>
       <c r="W26">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="X26">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
@@ -21526,11 +21516,11 @@
       </c>
       <c r="W27">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="X27">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
+        <v>0.69230769230769229</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
@@ -21562,18 +21552,18 @@
         <v>6</v>
       </c>
       <c r="Q28" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="V28">
         <v>27</v>
       </c>
       <c r="W28">
         <f>W27+(IF(ISNUMBER(O28),1,0))</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="X28">
         <f t="shared" si="1"/>
-        <v>0.77777777777777779</v>
+        <v>0.70370370370370372</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
@@ -21612,11 +21602,11 @@
       </c>
       <c r="W29">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X29">
         <f t="shared" si="1"/>
-        <v>0.7857142857142857</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
@@ -21652,11 +21642,11 @@
       </c>
       <c r="W30">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X30">
         <f t="shared" si="1"/>
-        <v>0.75862068965517238</v>
+        <v>0.68965517241379315</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
@@ -21692,11 +21682,11 @@
       </c>
       <c r="W31">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X31">
         <f t="shared" si="1"/>
-        <v>0.73333333333333328</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
@@ -21732,11 +21722,11 @@
       </c>
       <c r="W32">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X32">
         <f t="shared" si="1"/>
-        <v>0.70967741935483875</v>
+        <v>0.64516129032258063</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.3">
@@ -21768,18 +21758,18 @@
         <v>4</v>
       </c>
       <c r="Q33" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="V33">
         <v>32</v>
       </c>
       <c r="W33">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X33">
         <f t="shared" si="1"/>
-        <v>0.71875</v>
+        <v>0.65625</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
@@ -21812,18 +21802,18 @@
       </c>
       <c r="P34" s="7"/>
       <c r="Q34" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V34">
         <v>33</v>
       </c>
       <c r="W34">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X34">
         <f t="shared" si="1"/>
-        <v>0.69696969696969702</v>
+        <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
@@ -21856,18 +21846,18 @@
       </c>
       <c r="P35" s="7"/>
       <c r="Q35" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="V35">
         <v>34</v>
       </c>
       <c r="W35">
         <f t="shared" ref="W35:W66" si="2">W34+(IF(ISNUMBER(O35),1,0))</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X35">
         <f t="shared" si="1"/>
-        <v>0.67647058823529416</v>
+        <v>0.61764705882352944</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
@@ -21902,18 +21892,18 @@
         <v>1632</v>
       </c>
       <c r="Q36" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="V36">
         <v>35</v>
       </c>
       <c r="W36">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X36">
         <f t="shared" si="1"/>
-        <v>0.65714285714285714</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
@@ -21945,18 +21935,18 @@
         <v>1632</v>
       </c>
       <c r="Q37" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="V37">
         <v>36</v>
       </c>
       <c r="W37">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X37">
         <f t="shared" si="1"/>
-        <v>0.63888888888888884</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -21995,11 +21985,11 @@
       </c>
       <c r="W38">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="X38">
         <f t="shared" si="1"/>
-        <v>0.64864864864864868</v>
+        <v>0.59459459459459463</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
@@ -22035,11 +22025,11 @@
       </c>
       <c r="W39">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="X39">
         <f t="shared" si="1"/>
-        <v>0.65789473684210531</v>
+        <v>0.60526315789473684</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.3">
@@ -22072,18 +22062,18 @@
       </c>
       <c r="P40" s="7"/>
       <c r="Q40" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="V40">
         <v>39</v>
       </c>
       <c r="W40">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="X40">
         <f t="shared" si="1"/>
-        <v>0.64102564102564108</v>
+        <v>0.58974358974358976</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.3">
@@ -22119,11 +22109,11 @@
       </c>
       <c r="W41">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="X41">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.3">
@@ -22155,18 +22145,18 @@
         <v>1634</v>
       </c>
       <c r="Q42" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="V42">
         <v>41</v>
       </c>
       <c r="W42">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="X42">
         <f t="shared" si="1"/>
-        <v>0.6097560975609756</v>
+        <v>0.56097560975609762</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.3">
@@ -22202,11 +22192,11 @@
       </c>
       <c r="W43">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="X43">
         <f t="shared" si="1"/>
-        <v>0.59523809523809523</v>
+        <v>0.54761904761904767</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.3">
@@ -22242,11 +22232,11 @@
       </c>
       <c r="W44">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="X44">
         <f t="shared" si="1"/>
-        <v>0.58139534883720934</v>
+        <v>0.53488372093023251</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">
@@ -22274,8 +22264,8 @@
       <c r="M45" t="s">
         <v>96</v>
       </c>
-      <c r="O45" s="1">
-        <v>7</v>
+      <c r="O45" s="3">
+        <v>4</v>
       </c>
       <c r="P45" t="s">
         <v>1636</v>
@@ -22285,11 +22275,11 @@
       </c>
       <c r="W45">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X45">
         <f t="shared" si="1"/>
-        <v>0.59090909090909094</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.3">
@@ -22325,11 +22315,11 @@
       </c>
       <c r="W46">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X46">
         <f t="shared" si="1"/>
-        <v>0.57777777777777772</v>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.3">
@@ -22357,25 +22347,22 @@
       <c r="M47" t="s">
         <v>838</v>
       </c>
-      <c r="O47" s="6" t="s">
-        <v>1634</v>
-      </c>
-      <c r="P47" s="3">
+      <c r="O47" s="3">
         <v>13</v>
       </c>
       <c r="Q47" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="V47">
         <v>46</v>
       </c>
       <c r="W47">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f>W46+(IF(ISNUMBER(#REF!),1,0))</f>
+        <v>24</v>
       </c>
       <c r="X47">
         <f t="shared" si="1"/>
-        <v>0.56521739130434778</v>
+        <v>0.52173913043478259</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.3">
@@ -22411,11 +22398,11 @@
       </c>
       <c r="W48">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X48">
         <f t="shared" si="1"/>
-        <v>0.55319148936170215</v>
+        <v>0.51063829787234039</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.3">
@@ -22451,11 +22438,11 @@
       </c>
       <c r="W49">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X49">
         <f t="shared" si="1"/>
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
@@ -22491,11 +22478,11 @@
       </c>
       <c r="W50">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X50">
         <f t="shared" si="1"/>
-        <v>0.53061224489795922</v>
+        <v>0.48979591836734693</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.3">
@@ -22531,11 +22518,11 @@
       </c>
       <c r="W51">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="X51">
         <f t="shared" si="1"/>
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.3">
@@ -22571,11 +22558,11 @@
       </c>
       <c r="W52">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="X52">
         <f t="shared" si="1"/>
-        <v>0.52941176470588236</v>
+        <v>0.49019607843137253</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.3">
@@ -22611,11 +22598,11 @@
       </c>
       <c r="W53">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="X53">
         <f t="shared" si="1"/>
-        <v>0.51923076923076927</v>
+        <v>0.48076923076923078</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.3">
@@ -22651,11 +22638,11 @@
       </c>
       <c r="W54">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="X54">
         <f t="shared" si="1"/>
-        <v>0.50943396226415094</v>
+        <v>0.47169811320754718</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.3">
@@ -22694,11 +22681,11 @@
       </c>
       <c r="W55">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="X55">
         <f t="shared" si="1"/>
-        <v>0.51851851851851849</v>
+        <v>0.48148148148148145</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.3">
@@ -22730,18 +22717,18 @@
         <v>7</v>
       </c>
       <c r="P56" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="V56">
         <v>55</v>
       </c>
       <c r="W56">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X56">
         <f t="shared" si="1"/>
-        <v>0.52727272727272723</v>
+        <v>0.49090909090909091</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.3">
@@ -22773,18 +22760,18 @@
         <v>6</v>
       </c>
       <c r="Q57" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="V57">
         <v>56</v>
       </c>
       <c r="W57">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X57">
         <f t="shared" si="1"/>
-        <v>0.5357142857142857</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.3">
@@ -22820,11 +22807,11 @@
       </c>
       <c r="W58">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X58">
         <f t="shared" si="1"/>
-        <v>0.52631578947368418</v>
+        <v>0.49122807017543857</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.3">
@@ -22860,11 +22847,11 @@
       </c>
       <c r="W59">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X59">
         <f t="shared" si="1"/>
-        <v>0.51724137931034486</v>
+        <v>0.48275862068965519</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.3">
@@ -22900,11 +22887,11 @@
       </c>
       <c r="W60">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X60">
         <f t="shared" si="1"/>
-        <v>0.50847457627118642</v>
+        <v>0.47457627118644069</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.3">
@@ -22940,11 +22927,11 @@
       </c>
       <c r="W61">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X61">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
@@ -22980,11 +22967,11 @@
       </c>
       <c r="W62">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X62">
         <f t="shared" si="1"/>
-        <v>0.49180327868852458</v>
+        <v>0.45901639344262296</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.3">
@@ -23020,11 +23007,11 @@
       </c>
       <c r="W63">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X63">
         <f t="shared" si="1"/>
-        <v>0.4838709677419355</v>
+        <v>0.45161290322580644</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.3">
@@ -23060,11 +23047,11 @@
       </c>
       <c r="W64">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X64">
         <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.3">
@@ -23100,11 +23087,11 @@
       </c>
       <c r="W65">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X65">
         <f t="shared" si="1"/>
-        <v>0.46875</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.3">
@@ -23140,11 +23127,11 @@
       </c>
       <c r="W66">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X66">
         <f t="shared" si="1"/>
-        <v>0.46153846153846156</v>
+        <v>0.43076923076923079</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.3">
@@ -23180,11 +23167,11 @@
       </c>
       <c r="W67">
         <f t="shared" ref="W67:W101" si="3">W66+(IF(ISNUMBER(O67),1,0))</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X67">
         <f t="shared" ref="X67:X101" si="4">W67/V67</f>
-        <v>0.45454545454545453</v>
+        <v>0.42424242424242425</v>
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.3">
@@ -23220,11 +23207,11 @@
       </c>
       <c r="W68">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X68">
         <f t="shared" si="4"/>
-        <v>0.44776119402985076</v>
+        <v>0.41791044776119401</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.3">
@@ -23260,11 +23247,11 @@
       </c>
       <c r="W69">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X69">
         <f t="shared" si="4"/>
-        <v>0.44117647058823528</v>
+        <v>0.41176470588235292</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.3">
@@ -23296,18 +23283,18 @@
         <v>1632</v>
       </c>
       <c r="Q70" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="V70">
         <v>69</v>
       </c>
       <c r="W70">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X70">
         <f t="shared" si="4"/>
-        <v>0.43478260869565216</v>
+        <v>0.40579710144927539</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.3">
@@ -23339,18 +23326,18 @@
         <v>4</v>
       </c>
       <c r="Q71" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="V71">
         <v>70</v>
       </c>
       <c r="W71">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="X71">
         <f t="shared" si="4"/>
-        <v>0.44285714285714284</v>
+        <v>0.41428571428571431</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.3">
@@ -23386,11 +23373,11 @@
       </c>
       <c r="W72">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="X72">
         <f t="shared" si="4"/>
-        <v>0.43661971830985913</v>
+        <v>0.40845070422535212</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.3">
@@ -23426,11 +23413,11 @@
       </c>
       <c r="W73">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="X73">
         <f t="shared" si="4"/>
-        <v>0.44444444444444442</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.3">
@@ -23469,11 +23456,11 @@
       </c>
       <c r="W74">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X74">
         <f t="shared" si="4"/>
-        <v>0.45205479452054792</v>
+        <v>0.42465753424657532</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.3">
@@ -23506,18 +23493,18 @@
       </c>
       <c r="P75" s="7"/>
       <c r="Q75" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="V75">
         <v>74</v>
       </c>
       <c r="W75">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X75">
         <f t="shared" si="4"/>
-        <v>0.44594594594594594</v>
+        <v>0.41891891891891891</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.3">
@@ -23553,11 +23540,11 @@
       </c>
       <c r="W76">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X76">
         <f t="shared" si="4"/>
-        <v>0.44</v>
+        <v>0.41333333333333333</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.3">
@@ -23593,11 +23580,11 @@
       </c>
       <c r="W77">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X77">
         <f t="shared" si="4"/>
-        <v>0.44736842105263158</v>
+        <v>0.42105263157894735</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.3">
@@ -23633,11 +23620,11 @@
       </c>
       <c r="W78">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X78">
         <f t="shared" si="4"/>
-        <v>0.44155844155844154</v>
+        <v>0.41558441558441561</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.3">
@@ -23673,11 +23660,11 @@
       </c>
       <c r="W79">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X79">
         <f t="shared" si="4"/>
-        <v>0.4358974358974359</v>
+        <v>0.41025641025641024</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.3">
@@ -23713,11 +23700,11 @@
       </c>
       <c r="W80">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X80">
         <f t="shared" si="4"/>
-        <v>0.43037974683544306</v>
+        <v>0.4050632911392405</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.3">
@@ -23753,11 +23740,11 @@
       </c>
       <c r="W81">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X81">
         <f t="shared" si="4"/>
-        <v>0.42499999999999999</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.3">
@@ -23793,11 +23780,11 @@
       </c>
       <c r="W82">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X82">
         <f t="shared" si="4"/>
-        <v>0.41975308641975306</v>
+        <v>0.39506172839506171</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.3">
@@ -23833,11 +23820,11 @@
       </c>
       <c r="W83">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X83">
         <f t="shared" si="4"/>
-        <v>0.41463414634146339</v>
+        <v>0.3902439024390244</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.3">
@@ -23869,18 +23856,18 @@
         <v>6</v>
       </c>
       <c r="Q84" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="V84">
         <v>83</v>
       </c>
       <c r="W84">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="X84">
         <f t="shared" si="4"/>
-        <v>0.42168674698795183</v>
+        <v>0.39759036144578314</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.3">
@@ -23916,11 +23903,11 @@
       </c>
       <c r="W85">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="X85">
         <f t="shared" si="4"/>
-        <v>0.41666666666666669</v>
+        <v>0.39285714285714285</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.3">
@@ -23956,11 +23943,11 @@
       </c>
       <c r="W86">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="X86">
         <f t="shared" si="4"/>
-        <v>0.41176470588235292</v>
+        <v>0.38823529411764707</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.3">
@@ -23999,11 +23986,11 @@
       </c>
       <c r="W87">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X87">
         <f t="shared" si="4"/>
-        <v>0.41860465116279072</v>
+        <v>0.39534883720930231</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.3">
@@ -24035,18 +24022,18 @@
         <v>6</v>
       </c>
       <c r="Q88" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="V88">
         <v>87</v>
       </c>
       <c r="W88">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X88">
         <f t="shared" si="4"/>
-        <v>0.42528735632183906</v>
+        <v>0.40229885057471265</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.3">
@@ -24082,11 +24069,11 @@
       </c>
       <c r="W89">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X89">
         <f t="shared" si="4"/>
-        <v>0.42045454545454547</v>
+        <v>0.39772727272727271</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.3">
@@ -24122,11 +24109,11 @@
       </c>
       <c r="W90">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X90">
         <f t="shared" si="4"/>
-        <v>0.4157303370786517</v>
+        <v>0.39325842696629215</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.3">
@@ -24162,11 +24149,11 @@
       </c>
       <c r="W91">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X91">
         <f t="shared" si="4"/>
-        <v>0.41111111111111109</v>
+        <v>0.3888888888888889</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.3">
@@ -24202,11 +24189,11 @@
       </c>
       <c r="W92">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X92">
         <f t="shared" si="4"/>
-        <v>0.40659340659340659</v>
+        <v>0.38461538461538464</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.3">
@@ -24242,11 +24229,11 @@
       </c>
       <c r="W93">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X93">
         <f t="shared" si="4"/>
-        <v>0.40217391304347827</v>
+        <v>0.38043478260869568</v>
       </c>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.3">
@@ -24283,11 +24270,11 @@
       </c>
       <c r="W94">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X94">
         <f t="shared" si="4"/>
-        <v>0.39784946236559138</v>
+        <v>0.37634408602150538</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.3">
@@ -24323,11 +24310,11 @@
       </c>
       <c r="W95">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X95">
         <f t="shared" si="4"/>
-        <v>0.39361702127659576</v>
+        <v>0.37234042553191488</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.3">
@@ -24363,11 +24350,11 @@
       </c>
       <c r="W96">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X96">
         <f t="shared" si="4"/>
-        <v>0.38947368421052631</v>
+        <v>0.36842105263157893</v>
       </c>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.3">
@@ -24403,11 +24390,11 @@
       </c>
       <c r="W97">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X97">
         <f t="shared" si="4"/>
-        <v>0.38541666666666669</v>
+        <v>0.36458333333333331</v>
       </c>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.3">
@@ -24443,11 +24430,11 @@
       </c>
       <c r="W98">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X98">
         <f t="shared" si="4"/>
-        <v>0.38144329896907214</v>
+        <v>0.36082474226804123</v>
       </c>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.3">
@@ -24482,18 +24469,18 @@
         <v>1634</v>
       </c>
       <c r="Q99" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="V99">
         <v>98</v>
       </c>
       <c r="W99">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="X99">
         <f t="shared" si="4"/>
-        <v>0.38775510204081631</v>
+        <v>0.36734693877551022</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.3">
@@ -24529,11 +24516,11 @@
       </c>
       <c r="W100">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="X100">
         <f t="shared" si="4"/>
-        <v>0.38383838383838381</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.3">
@@ -24569,11 +24556,11 @@
       </c>
       <c r="W101">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="X101">
         <f t="shared" si="4"/>
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.3">
@@ -24687,7 +24674,7 @@
       </c>
       <c r="P105" s="7"/>
       <c r="Q105" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.3">
@@ -33187,7 +33174,7 @@
         <v>7</v>
       </c>
       <c r="Q431" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="432" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>